<commit_message>
Tablas y ejercicios de bases de datos
</commit_message>
<xml_diff>
--- a/Ejercicios/Ejercicios/LenguajeAvanzado/ExClosedXML/CsvConverter/converter.xlsx
+++ b/Ejercicios/Ejercicios/LenguajeAvanzado/ExClosedXML/CsvConverter/converter.xlsx
@@ -19,19 +19,19 @@
     <x:t>Nombre</x:t>
   </x:si>
   <x:si>
-    <x:t>Contraseña</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ContraseñaHash</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Edad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Banco</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Saldo</x:t>
+    <x:t xml:space="preserve"> Contraseña</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Contraseña Hash</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Edad</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Banco</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Saldo</x:t>
   </x:si>
   <x:si>
     <x:t>Alfred</x:t>
@@ -43,9 +43,15 @@
     <x:t>C37BF859FAF392800D739A41FE5AF151</x:t>
   </x:si>
   <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
     <x:t>Santander</x:t>
   </x:si>
   <x:si>
+    <x:t>1000</x:t>
+  </x:si>
+  <x:si>
     <x:t>Juan</x:t>
   </x:si>
   <x:si>
@@ -58,6 +64,9 @@
     <x:t>Ibercaja</x:t>
   </x:si>
   <x:si>
+    <x:t>2000</x:t>
+  </x:si>
+  <x:si>
     <x:t>Pepito</x:t>
   </x:si>
   <x:si>
@@ -70,6 +79,9 @@
     <x:t>BBVA</x:t>
   </x:si>
   <x:si>
+    <x:t>10000</x:t>
+  </x:si>
+  <x:si>
     <x:t>Laura</x:t>
   </x:si>
   <x:si>
@@ -79,6 +91,9 @@
     <x:t>992A6D18B2A148CF20D9014C3524AA11</x:t>
   </x:si>
   <x:si>
+    <x:t>500</x:t>
+  </x:si>
+  <x:si>
     <x:t>Alberto</x:t>
   </x:si>
   <x:si>
@@ -88,6 +103,9 @@
     <x:t>01CFCD4F6B8770FEBFB40CB906715822</x:t>
   </x:si>
   <x:si>
+    <x:t>100</x:t>
+  </x:si>
+  <x:si>
     <x:t>Alvaro</x:t>
   </x:si>
   <x:si>
@@ -98,6 +116,9 @@
   </x:si>
   <x:si>
     <x:t>BancoPixinxa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5000</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -448,13 +469,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F7"/>
+  <x:dimension ref="A1:G7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -474,7 +495,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
+    <x:row r="2" spans="1:7">
       <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -484,114 +505,114 @@
       <x:c r="C2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D2" s="0">
+      <x:c r="D2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="A5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F2" s="0">
-        <x:v>1000</x:v>
+      <x:c r="E5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
+    <x:row r="6" spans="1:7">
+      <x:c r="A6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D3" s="0">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="F3" s="0">
-        <x:v>2000</x:v>
+      <x:c r="F6" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D4" s="0">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F4" s="0">
-        <x:v>10000</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6">
-      <x:c r="A5" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D5" s="0">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F5" s="0">
-        <x:v>500</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:6">
-      <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D6" s="0">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
+    <x:row r="7" spans="1:7">
+      <x:c r="A7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F6" s="0">
-        <x:v>100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6">
-      <x:c r="A7" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="D7" s="0">
-        <x:v>23</x:v>
-      </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F7" s="0">
-        <x:v>5000</x:v>
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>